<commit_message>
Updates to the custom plots functions
</commit_message>
<xml_diff>
--- a/CustomPlots/VelocityTuning_Plot_Def.xlsx
+++ b/CustomPlots/VelocityTuning_Plot_Def.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matt\Documents\kVIS3_bsp_ardupilot\CustomPlots\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7B40DE-598B-4191-B32F-2928C8461A25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2754E02-1A01-4953-BC30-136C74F465A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
+    <workbookView xWindow="3105" yWindow="1170" windowWidth="23685" windowHeight="13545" xr2:uid="{BA9E8F30-6C98-CF4B-8E95-183011E815A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="60">
   <si>
     <t>KSID Custom Plot Definition</t>
   </si>
@@ -187,6 +189,30 @@
   </si>
   <si>
     <t>VelocityTuning</t>
+  </si>
+  <si>
+    <t>PL/vX</t>
+  </si>
+  <si>
+    <t>PL/vY</t>
+  </si>
+  <si>
+    <t>PL/pX</t>
+  </si>
+  <si>
+    <t>PL/pY</t>
+  </si>
+  <si>
+    <t>VN_{PrecLand}</t>
+  </si>
+  <si>
+    <t>PE_{PrecLand}</t>
+  </si>
+  <si>
+    <t>VE_{PrecLand}</t>
+  </si>
+  <si>
+    <t>PN_{PrecLand}</t>
   </si>
 </sst>
 </file>
@@ -550,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7D595D-48C5-5044-8E94-F6ADF0970571}">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -562,7 +588,9 @@
     <col min="8" max="8" width="15.625" customWidth="1"/>
     <col min="10" max="10" width="20.125" customWidth="1"/>
     <col min="11" max="11" width="30.5" customWidth="1"/>
-    <col min="12" max="12" width="18.5" customWidth="1"/>
+    <col min="12" max="12" width="4.875" customWidth="1"/>
+    <col min="13" max="13" width="4.625" customWidth="1"/>
+    <col min="14" max="14" width="5.125" customWidth="1"/>
     <col min="15" max="15" width="13.875" customWidth="1"/>
     <col min="16" max="16" width="16.5" customWidth="1"/>
     <col min="17" max="17" width="16.375" customWidth="1"/>
@@ -727,7 +755,7 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8">
         <v>2</v>
@@ -742,22 +770,22 @@
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="O8">
-        <v>1</v>
+        <v>-0.01</v>
       </c>
       <c r="R8" t="s">
-        <v>38</v>
+        <v>56</v>
       </c>
       <c r="S8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -783,13 +811,13 @@
         <v>24</v>
       </c>
       <c r="K9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O9">
         <v>1</v>
       </c>
       <c r="R9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S9" t="s">
         <v>25</v>
@@ -818,13 +846,13 @@
         <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
       <c r="R10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="S10" t="s">
         <v>25</v>
@@ -832,13 +860,13 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
@@ -847,33 +875,33 @@
         <v>23</v>
       </c>
       <c r="F11" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
       </c>
       <c r="K11" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>-0.01</v>
       </c>
       <c r="R11" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="S11" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>2</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>18</v>
@@ -882,27 +910,27 @@
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="O12">
         <v>1</v>
       </c>
       <c r="R12" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="S12" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -917,27 +945,27 @@
         <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
       </c>
       <c r="K13" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="O13">
         <v>1</v>
       </c>
       <c r="R13" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="S13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -952,56 +980,196 @@
         <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G14" t="s">
         <v>24</v>
       </c>
       <c r="K14" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="O14">
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="S14" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" t="s">
+        <v>53</v>
+      </c>
+      <c r="O15">
+        <v>-0.01</v>
+      </c>
+      <c r="R15" t="s">
+        <v>58</v>
+      </c>
+      <c r="S15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>4</v>
       </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" t="s">
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
         <v>37</v>
       </c>
-      <c r="G15" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="G16" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" t="s">
+        <v>43</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>45</v>
+      </c>
+      <c r="S16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
+      </c>
+      <c r="K17" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>46</v>
+      </c>
+      <c r="S17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" t="s">
+        <v>24</v>
+      </c>
+      <c r="K18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O18">
+        <v>-0.01</v>
+      </c>
+      <c r="R18" t="s">
+        <v>57</v>
+      </c>
+      <c r="S18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19" t="s">
         <v>49</v>
       </c>
-      <c r="O15">
-        <v>1</v>
-      </c>
-      <c r="R15" t="s">
+      <c r="O19">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
         <v>48</v>
       </c>
-      <c r="S15" t="s">
+      <c r="S19" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>